<commit_message>
adding no data for aggravating
</commit_message>
<xml_diff>
--- a/input/Template_EMIS_Access_PTR_protection.xlsx
+++ b/input/Template_EMIS_Access_PTR_protection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted-my.sharepoint.com/personal/martina_vit_impact-initiatives_org/Documents/PiN_app_dev/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="443" documentId="8_{D63770E9-8D5C-4F2A-BD7D-98D3C6683B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB93B9E7-FCAA-4092-9779-2202E5EB6006}"/>
+  <xr:revisionPtr revIDLastSave="469" documentId="8_{D63770E9-8D5C-4F2A-BD7D-98D3C6683B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B793117-7AB4-49DD-B3A2-3AEDF5B7A79E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{24D09A16-471A-4A7F-BD10-C475AB78837D}"/>
+    <workbookView xWindow="28905" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{24D09A16-471A-4A7F-BD10-C475AB78837D}"/>
   </bookViews>
   <sheets>
     <sheet name="indicator" sheetId="3" r:id="rId1"/>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Admin Pcode</t>
   </si>
@@ -124,6 +124,18 @@
   </si>
   <si>
     <t>threshold PTR (Change it according to the context average PTR)</t>
+  </si>
+  <si>
+    <t>Protection indicator value -- categorical variable</t>
+  </si>
+  <si>
+    <t>Protection indicator value -- continuous / discrete numerical variable</t>
+  </si>
+  <si>
+    <t>category for categorical variable --&gt; if selected the child is in need</t>
+  </si>
+  <si>
+    <t>threshold for numerical variable --&gt; if above the child is in need</t>
   </si>
 </sst>
 </file>
@@ -179,7 +191,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -190,6 +202,19 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
       </patternFill>
+    </fill>
+    <fill>
+      <gradientFill degree="135">
+        <stop position="0">
+          <color theme="0"/>
+        </stop>
+        <stop position="0.5">
+          <color rgb="FFFFFFCC"/>
+        </stop>
+        <stop position="1">
+          <color theme="0"/>
+        </stop>
+      </gradientFill>
     </fill>
   </fills>
   <borders count="2">
@@ -221,7 +246,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -239,6 +264,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17DEB9B6-621B-4484-8A08-69293BE9C3A3}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,10 +623,14 @@
     <col min="5" max="5" width="10.28515625" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" style="6" customWidth="1"/>
     <col min="7" max="7" width="37" style="6" customWidth="1"/>
-    <col min="8" max="10" width="22.85546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" style="8" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" style="8" customWidth="1"/>
+    <col min="10" max="10" width="23.5703125" style="8" customWidth="1"/>
+    <col min="11" max="11" width="25.140625" style="8" customWidth="1"/>
+    <col min="12" max="14" width="22.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -619,18 +652,30 @@
       <c r="G1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
     </row>
   </sheetData>
   <protectedRanges>

</xml_diff>